<commit_message>
First Commit - Migrating to SQLite database. Added script to setup database.
</commit_message>
<xml_diff>
--- a/public/sheets/kids.xlsx
+++ b/public/sheets/kids.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scian\Documents\Projects\afterschool-api\public\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7A6F2A-BFB4-47F6-B471-DC7E27AFFF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42798557-20EE-4631-AF71-7F3400C88FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1575" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1575" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kids" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -105,12 +105,6 @@
     <t>Relationship</t>
   </si>
   <si>
-    <t>Ids</t>
-  </si>
-  <si>
-    <t>1, 5, 6</t>
-  </si>
-  <si>
     <t>paul@example.com</t>
   </si>
   <si>
@@ -145,6 +139,12 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>Guardians</t>
+  </si>
+  <si>
+    <t>1, 2</t>
   </si>
 </sst>
 </file>
@@ -231,7 +231,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -239,10 +239,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -546,15 +549,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -567,8 +570,11 @@
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -581,8 +587,11 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -595,8 +604,11 @@
       <c r="D3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
@@ -609,8 +621,11 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7</v>
       </c>
@@ -623,8 +638,11 @@
       <c r="D5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8</v>
       </c>
@@ -635,6 +653,9 @@
         <v>22</v>
       </c>
       <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6">
         <v>4</v>
       </c>
     </row>
@@ -647,15 +668,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AA94AF8-4C84-4B99-B4AE-10B00DC34FD6}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -674,8 +695,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>28</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -684,18 +705,18 @@
         <v>98274092</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>28</v>
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -704,53 +725,53 @@
         <v>92348574</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
         <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4">
         <v>82345093</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
         <v>35</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>37</v>
-      </c>
-      <c r="F4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5">
         <v>23458909</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
         <v>36</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>38</v>
-      </c>
-      <c r="F5" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>